<commit_message>
RN-1161: Retain service type for tupaia data elements on survey reimport
</commit_message>
<xml_diff>
--- a/packages/central-server/src/tests/testData/surveys/importANewSurvey.xlsx
+++ b/packages/central-server/src/tests/testData/surveys/importANewSurvey.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects\tupaia\packages\meditrak-server\src\tests\testData\surveys\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C384F0-470A-4A55-B165-844296EE0D04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="new_survey_import_1_test" sheetId="2" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="new_survey_import_1_test"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,16 +61,16 @@
     <t>detailLabel</t>
   </si>
   <si>
+    <t>fdfuu42a22321c123a8_test_new</t>
+  </si>
+  <si>
     <t>FreeText</t>
   </si>
   <si>
-    <t>fdfuu42a22321c123a8_test</t>
-  </si>
-  <si>
     <t>Test question fdfuu42a22321c123a8_test</t>
   </si>
   <si>
-    <t>fdfzz42a66321c123a8_test</t>
+    <t>fdfzz42a66321c123a8_test_new</t>
   </si>
   <si>
     <t>Test question fdfzz42a66321c123a8_test</t>
@@ -85,10 +79,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -115,42 +110,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -161,10 +137,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -202,71 +178,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -290,50 +266,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -343,7 +322,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -352,7 +331,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -361,7 +340,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -369,10 +348,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -401,7 +380,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -414,13 +393,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -432,61 +410,40 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91190F5A-C39F-47E3-9B71-45A0A62043BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="57.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,12 +490,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -558,12 +515,12 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -583,7 +540,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -601,13 +558,6 @@
       <c r="O4" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A4">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RN-1161: Retain service type for tupaia data elements on survey reimport (#5410)
* RN-1161: Retain service type for tupaia data elements on survey reimport

* Rename method

* rename file

* Fix issue with config not carrying over

* Fix early return

* FIx regression

---------

Co-authored-by: Andrew <vanbeekandrew@gmail.com>
</commit_message>
<xml_diff>
--- a/packages/central-server/src/tests/testData/surveys/importANewSurvey.xlsx
+++ b/packages/central-server/src/tests/testData/surveys/importANewSurvey.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects\tupaia\packages\meditrak-server\src\tests\testData\surveys\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C384F0-470A-4A55-B165-844296EE0D04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="new_survey_import_1_test" sheetId="2" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="new_survey_import_1_test"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,16 +61,16 @@
     <t>detailLabel</t>
   </si>
   <si>
+    <t>fdfuu42a22321c123a8_test_new</t>
+  </si>
+  <si>
     <t>FreeText</t>
   </si>
   <si>
-    <t>fdfuu42a22321c123a8_test</t>
-  </si>
-  <si>
     <t>Test question fdfuu42a22321c123a8_test</t>
   </si>
   <si>
-    <t>fdfzz42a66321c123a8_test</t>
+    <t>fdfzz42a66321c123a8_test_new</t>
   </si>
   <si>
     <t>Test question fdfzz42a66321c123a8_test</t>
@@ -85,10 +79,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -115,42 +110,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -161,10 +137,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -202,71 +178,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -290,50 +266,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -343,7 +322,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -352,7 +331,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -361,7 +340,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -369,10 +348,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -401,7 +380,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -414,13 +393,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -432,61 +410,40 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91190F5A-C39F-47E3-9B71-45A0A62043BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="57.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,12 +490,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -558,12 +515,12 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -583,7 +540,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -601,13 +558,6 @@
       <c r="O4" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A4">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>